<commit_message>
Updated sheet for multi stock watchlist
</commit_message>
<xml_diff>
--- a/Stock_Value_alert.xlsx
+++ b/Stock_Value_alert.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Stock Name</t>
   </si>
   <si>
-    <t>Tata Motors Limited</t>
-  </si>
-  <si>
     <t>Live Price</t>
   </si>
   <si>
@@ -31,6 +28,87 @@
   </si>
   <si>
     <t>Value Difference</t>
+  </si>
+  <si>
+    <t>TATAMOTORS.NS</t>
+  </si>
+  <si>
+    <t>RELIANCE.NS</t>
+  </si>
+  <si>
+    <t>SBIN.NS</t>
+  </si>
+  <si>
+    <t>ASIANPAINT.NS</t>
+  </si>
+  <si>
+    <t>AMARAJABAT.NS</t>
+  </si>
+  <si>
+    <t>HDFCBANK.NS</t>
+  </si>
+  <si>
+    <t>KOTAKBANK.NS</t>
+  </si>
+  <si>
+    <t>TITAN.NS</t>
+  </si>
+  <si>
+    <t>TCS.NS</t>
+  </si>
+  <si>
+    <t>BHARATRAS.NS</t>
+  </si>
+  <si>
+    <t>MARICO.NS</t>
+  </si>
+  <si>
+    <t>HINDUNILVR.NS</t>
+  </si>
+  <si>
+    <t>PIDILITIND.NS</t>
+  </si>
+  <si>
+    <t>NESTLEIND.NS</t>
+  </si>
+  <si>
+    <t>HCLTECH.NS</t>
+  </si>
+  <si>
+    <t>BRITANNIA.NS</t>
+  </si>
+  <si>
+    <t>BERGEPAINT.NS</t>
+  </si>
+  <si>
+    <t>MOTHERSUMI.NS</t>
+  </si>
+  <si>
+    <t>BALKRISIND.NS</t>
+  </si>
+  <si>
+    <t>MINDTREE.NS</t>
+  </si>
+  <si>
+    <t>ASTRAL.NS</t>
+  </si>
+  <si>
+    <t>TATAPOWER.NS</t>
+  </si>
+  <si>
+    <t>TATACHEM.NS</t>
+  </si>
+  <si>
+    <t>ITC.NS</t>
+  </si>
+  <si>
+    <t>TATACONSUM.NS</t>
+  </si>
+  <si>
+    <t>GODREJCP.NS</t>
+  </si>
+  <si>
+    <t>Response Time</t>
   </si>
 </sst>
 </file>
@@ -74,9 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,48 +457,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1">
+        <v>-55.013939999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="B2">
-        <v>341.85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>344.9</v>
+      </c>
+      <c r="C2">
+        <v>340</v>
+      </c>
+      <c r="D2">
+        <v>4.8999999999999773</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+        <v>2129.0500000000002</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+      <c r="D3">
+        <v>129.05000000000018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3005</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>746.55</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>746.55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1480.4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1480.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>1715.15</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1715.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1754.75</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1754.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>3325.45</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3325.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>13620.8</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>13620.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>519.85</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>519.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>2487.3000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2487.3000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>2178.85</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2178.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>17602</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>17602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>984.65</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>984.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>3545.3</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>3545.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>806.9</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>806.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>245.4</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>245.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>2298.85</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2298.85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>2583.1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>2583.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>2040.8</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2040.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>424.4</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>424.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>120.95</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>120.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>1.8500000000000227</v>
+      <c r="B24">
+        <v>344.9</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>344.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>767.7</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>767.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>202.4</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>202.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>763.6</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>763.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>891.25</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>891.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>